<commit_message>
The Purchase Order module is updated:
The starting and offsetting percentage is added
</commit_message>
<xml_diff>
--- a/static/documentos/orden_compra.xlsx
+++ b/static/documentos/orden_compra.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\PycharmProjects\uni2data\static\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC63DEB-5F52-418B-BA3D-CA359BEE5F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78683A9B-6B86-4890-8FEA-22723100180C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BCC1EEF9-1AB8-4B02-AD3B-A548C56B21AA}"/>
   </bookViews>
@@ -192,14 +192,6 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color theme="8" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="16"/>
       <color theme="4" tint="0.39997558519241921"/>
       <name val="Arial Black"/>
@@ -212,6 +204,13 @@
       <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -558,12 +557,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -598,7 +591,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -619,70 +612,198 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="7" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="7" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -698,187 +819,65 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="7" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="7" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="2" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="2" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="3" fillId="5" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="3" fillId="5" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="2" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="2" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1199,99 +1198,99 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF2228A2-6696-4731-9F07-396E6E27E4B6}">
   <dimension ref="A2:J55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54:F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
     <col min="7" max="7" width="7.85546875" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" customWidth="1"/>
     <col min="9" max="9" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="125"/>
-      <c r="C2" s="126"/>
-      <c r="D2" s="127"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="89"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="58"/>
     </row>
     <row r="3" spans="1:10" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="73"/>
-      <c r="C3" s="128"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="92"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="61"/>
     </row>
     <row r="4" spans="1:10" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
-      <c r="B4" s="129"/>
-      <c r="C4" s="130"/>
-      <c r="D4" s="131"/>
-      <c r="E4" s="93"/>
-      <c r="F4" s="94"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="94"/>
-      <c r="I4" s="94"/>
-      <c r="J4" s="95"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="64"/>
     </row>
     <row r="5" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="33" t="s">
+      <c r="F5" s="34"/>
+      <c r="G5" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="33"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="37"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="35"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
-      <c r="B6" s="101" t="s">
+      <c r="B6" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="102"/>
-      <c r="D6" s="135"/>
-      <c r="E6" s="135"/>
-      <c r="F6" s="135"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="92"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="92"/>
       <c r="G6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="103"/>
-      <c r="I6" s="104"/>
-      <c r="J6" s="39"/>
+      <c r="H6" s="81"/>
+      <c r="I6" s="82"/>
+      <c r="J6" s="37"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
-      <c r="B7" s="101" t="s">
+      <c r="B7" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="102"/>
-      <c r="D7" s="135"/>
-      <c r="E7" s="135"/>
-      <c r="F7" s="135"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="92"/>
       <c r="G7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="105"/>
-      <c r="I7" s="106"/>
-      <c r="J7" s="39"/>
+      <c r="H7" s="83"/>
+      <c r="I7" s="84"/>
+      <c r="J7" s="37"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
@@ -1299,100 +1298,100 @@
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
       <c r="H8" s="18"/>
       <c r="I8" s="18"/>
-      <c r="J8" s="40"/>
+      <c r="J8" s="38"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="96" t="s">
+      <c r="B9" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="97"/>
-      <c r="D9" s="97"/>
-      <c r="E9" s="97"/>
-      <c r="F9" s="97"/>
-      <c r="G9" s="97"/>
-      <c r="H9" s="97" t="s">
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="97"/>
-      <c r="J9" s="97"/>
+      <c r="I9" s="66"/>
+      <c r="J9" s="66"/>
     </row>
     <row r="10" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="107" t="s">
+      <c r="B10" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="108"/>
-      <c r="D10" s="107"/>
-      <c r="E10" s="132"/>
-      <c r="F10" s="132"/>
-      <c r="G10" s="108"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="37"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="89"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="86"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="35"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="109" t="s">
+      <c r="B11" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="110"/>
-      <c r="D11" s="109"/>
-      <c r="E11" s="133"/>
-      <c r="F11" s="133"/>
-      <c r="G11" s="110"/>
-      <c r="H11" s="98"/>
-      <c r="I11" s="99"/>
-      <c r="J11" s="100"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="87"/>
+      <c r="E11" s="90"/>
+      <c r="F11" s="90"/>
+      <c r="G11" s="88"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="68"/>
+      <c r="J11" s="69"/>
     </row>
     <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="109" t="s">
+      <c r="B12" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="110"/>
-      <c r="D12" s="109"/>
-      <c r="E12" s="133"/>
-      <c r="F12" s="133"/>
-      <c r="G12" s="110"/>
-      <c r="H12" s="98"/>
-      <c r="I12" s="99"/>
-      <c r="J12" s="100"/>
+      <c r="C12" s="88"/>
+      <c r="D12" s="87"/>
+      <c r="E12" s="90"/>
+      <c r="F12" s="90"/>
+      <c r="G12" s="88"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="68"/>
+      <c r="J12" s="69"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="85" t="s">
+      <c r="B13" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="86"/>
-      <c r="D13" s="85"/>
-      <c r="E13" s="134"/>
-      <c r="F13" s="134"/>
-      <c r="G13" s="86"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="40"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="91"/>
+      <c r="F13" s="91"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="38"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B14" s="43"/>
+      <c r="B14" s="41"/>
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
       <c r="F14" s="20"/>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="37"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="35"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="26"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
       <c r="I15" s="16"/>
-      <c r="J15" s="39"/>
+      <c r="J15" s="37"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="11"/>
@@ -1403,37 +1402,37 @@
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
       <c r="I16" s="16"/>
-      <c r="J16" s="39"/>
+      <c r="J16" s="37"/>
     </row>
     <row r="17" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="83" t="s">
+      <c r="C17" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="83"/>
-      <c r="E17" s="83"/>
-      <c r="F17" s="83"/>
+      <c r="D17" s="103"/>
+      <c r="E17" s="103"/>
+      <c r="F17" s="103"/>
       <c r="G17" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="38"/>
     </row>
     <row r="18" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
-      <c r="C18" s="84" t="s">
+      <c r="C18" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="84"/>
-      <c r="E18" s="84"/>
-      <c r="F18" s="84"/>
+      <c r="D18" s="104"/>
+      <c r="E18" s="104"/>
+      <c r="F18" s="104"/>
       <c r="G18" s="9"/>
       <c r="H18" s="15"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="39"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="37"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
@@ -1443,335 +1442,335 @@
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="40"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="38"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="63" t="s">
+      <c r="B20" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="28" t="s">
+      <c r="C20" s="114"/>
+      <c r="D20" s="114"/>
+      <c r="E20" s="106"/>
+      <c r="F20" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="63" t="s">
+      <c r="G20" s="105" t="s">
         <v>17</v>
       </c>
-      <c r="H20" s="65"/>
-      <c r="I20" s="63" t="s">
+      <c r="H20" s="106"/>
+      <c r="I20" s="105" t="s">
         <v>18</v>
       </c>
-      <c r="J20" s="65"/>
+      <c r="J20" s="106"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="66"/>
-      <c r="C21" s="67"/>
-      <c r="D21" s="67"/>
-      <c r="E21" s="68"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="119"/>
-      <c r="H21" s="120"/>
+      <c r="B21" s="115"/>
+      <c r="C21" s="116"/>
+      <c r="D21" s="116"/>
+      <c r="E21" s="117"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="47"/>
       <c r="I21" s="73"/>
-      <c r="J21" s="74"/>
+      <c r="J21" s="75"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="44"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="119"/>
-      <c r="H22" s="120"/>
+      <c r="B22" s="118"/>
+      <c r="C22" s="119"/>
+      <c r="D22" s="119"/>
+      <c r="E22" s="120"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="47"/>
       <c r="I22" s="73"/>
-      <c r="J22" s="74"/>
+      <c r="J22" s="75"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="44"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="69"/>
-      <c r="H23" s="70"/>
+      <c r="B23" s="118"/>
+      <c r="C23" s="119"/>
+      <c r="D23" s="119"/>
+      <c r="E23" s="120"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="49"/>
       <c r="I23" s="73"/>
-      <c r="J23" s="74"/>
+      <c r="J23" s="75"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="44"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="69"/>
-      <c r="H24" s="70"/>
+      <c r="B24" s="118"/>
+      <c r="C24" s="119"/>
+      <c r="D24" s="119"/>
+      <c r="E24" s="120"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="49"/>
       <c r="I24" s="73"/>
-      <c r="J24" s="74"/>
+      <c r="J24" s="75"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="44"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="69"/>
-      <c r="H25" s="70"/>
+      <c r="B25" s="118"/>
+      <c r="C25" s="119"/>
+      <c r="D25" s="119"/>
+      <c r="E25" s="120"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="49"/>
       <c r="I25" s="73"/>
-      <c r="J25" s="74"/>
+      <c r="J25" s="75"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="44"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="69"/>
-      <c r="H26" s="70"/>
+      <c r="B26" s="118"/>
+      <c r="C26" s="119"/>
+      <c r="D26" s="119"/>
+      <c r="E26" s="120"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="49"/>
       <c r="I26" s="73"/>
-      <c r="J26" s="74"/>
+      <c r="J26" s="75"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="44"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="69"/>
-      <c r="H27" s="70"/>
+      <c r="B27" s="118"/>
+      <c r="C27" s="119"/>
+      <c r="D27" s="119"/>
+      <c r="E27" s="120"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="49"/>
       <c r="I27" s="73"/>
-      <c r="J27" s="74"/>
+      <c r="J27" s="75"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="44"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="46"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="69"/>
-      <c r="H28" s="70"/>
+      <c r="B28" s="118"/>
+      <c r="C28" s="119"/>
+      <c r="D28" s="119"/>
+      <c r="E28" s="120"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="49"/>
       <c r="I28" s="73"/>
-      <c r="J28" s="74"/>
+      <c r="J28" s="75"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="44"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="69"/>
-      <c r="H29" s="70"/>
+      <c r="B29" s="118"/>
+      <c r="C29" s="119"/>
+      <c r="D29" s="119"/>
+      <c r="E29" s="120"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="48"/>
+      <c r="H29" s="49"/>
       <c r="I29" s="73"/>
-      <c r="J29" s="74"/>
+      <c r="J29" s="75"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="44"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="69"/>
-      <c r="H30" s="70"/>
+      <c r="B30" s="118"/>
+      <c r="C30" s="119"/>
+      <c r="D30" s="119"/>
+      <c r="E30" s="120"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="49"/>
       <c r="I30" s="73"/>
-      <c r="J30" s="74"/>
+      <c r="J30" s="75"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="44"/>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="69"/>
-      <c r="H31" s="70"/>
+      <c r="B31" s="118"/>
+      <c r="C31" s="119"/>
+      <c r="D31" s="119"/>
+      <c r="E31" s="120"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="49"/>
       <c r="I31" s="73"/>
-      <c r="J31" s="74"/>
+      <c r="J31" s="75"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="44"/>
-      <c r="C32" s="45"/>
-      <c r="D32" s="45"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="69"/>
-      <c r="H32" s="70"/>
+      <c r="B32" s="118"/>
+      <c r="C32" s="119"/>
+      <c r="D32" s="119"/>
+      <c r="E32" s="120"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="48"/>
+      <c r="H32" s="49"/>
       <c r="I32" s="73"/>
-      <c r="J32" s="74"/>
+      <c r="J32" s="75"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="44"/>
-      <c r="C33" s="45"/>
-      <c r="D33" s="45"/>
-      <c r="E33" s="46"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="69"/>
-      <c r="H33" s="70"/>
+      <c r="B33" s="118"/>
+      <c r="C33" s="119"/>
+      <c r="D33" s="119"/>
+      <c r="E33" s="120"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="48"/>
+      <c r="H33" s="49"/>
       <c r="I33" s="73"/>
-      <c r="J33" s="74"/>
+      <c r="J33" s="75"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="44"/>
-      <c r="C34" s="45"/>
-      <c r="D34" s="45"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="69"/>
-      <c r="H34" s="70"/>
+      <c r="B34" s="118"/>
+      <c r="C34" s="119"/>
+      <c r="D34" s="119"/>
+      <c r="E34" s="120"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="49"/>
       <c r="I34" s="73"/>
-      <c r="J34" s="74"/>
+      <c r="J34" s="75"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="44"/>
-      <c r="C35" s="45"/>
-      <c r="D35" s="45"/>
-      <c r="E35" s="46"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="69"/>
-      <c r="H35" s="70"/>
+      <c r="B35" s="118"/>
+      <c r="C35" s="119"/>
+      <c r="D35" s="119"/>
+      <c r="E35" s="120"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="48"/>
+      <c r="H35" s="49"/>
       <c r="I35" s="73"/>
-      <c r="J35" s="74"/>
+      <c r="J35" s="75"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="44"/>
-      <c r="C36" s="45"/>
-      <c r="D36" s="45"/>
-      <c r="E36" s="46"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="69"/>
-      <c r="H36" s="70"/>
-      <c r="I36" s="71"/>
-      <c r="J36" s="72"/>
+      <c r="B36" s="118"/>
+      <c r="C36" s="119"/>
+      <c r="D36" s="119"/>
+      <c r="E36" s="120"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="48"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="107"/>
+      <c r="J36" s="108"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="44"/>
-      <c r="C37" s="45"/>
-      <c r="D37" s="45"/>
-      <c r="E37" s="46"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="69"/>
-      <c r="H37" s="70"/>
-      <c r="I37" s="71"/>
-      <c r="J37" s="72"/>
+      <c r="B37" s="118"/>
+      <c r="C37" s="119"/>
+      <c r="D37" s="119"/>
+      <c r="E37" s="120"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="48"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="107"/>
+      <c r="J37" s="108"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="44"/>
-      <c r="C38" s="45"/>
-      <c r="D38" s="45"/>
-      <c r="E38" s="46"/>
-      <c r="F38" s="32"/>
-      <c r="G38" s="69"/>
-      <c r="H38" s="70"/>
-      <c r="I38" s="71"/>
-      <c r="J38" s="72"/>
+      <c r="B38" s="118"/>
+      <c r="C38" s="119"/>
+      <c r="D38" s="119"/>
+      <c r="E38" s="120"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="48"/>
+      <c r="H38" s="49"/>
+      <c r="I38" s="107"/>
+      <c r="J38" s="108"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="44"/>
-      <c r="C39" s="45"/>
-      <c r="D39" s="45"/>
-      <c r="E39" s="46"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="69"/>
-      <c r="H39" s="70"/>
-      <c r="I39" s="71"/>
-      <c r="J39" s="72"/>
+      <c r="B39" s="118"/>
+      <c r="C39" s="119"/>
+      <c r="D39" s="119"/>
+      <c r="E39" s="120"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="48"/>
+      <c r="H39" s="49"/>
+      <c r="I39" s="107"/>
+      <c r="J39" s="108"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="44"/>
-      <c r="C40" s="45"/>
-      <c r="D40" s="45"/>
-      <c r="E40" s="46"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="69"/>
-      <c r="H40" s="70"/>
-      <c r="I40" s="71"/>
-      <c r="J40" s="72"/>
+      <c r="B40" s="118"/>
+      <c r="C40" s="119"/>
+      <c r="D40" s="119"/>
+      <c r="E40" s="120"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="48"/>
+      <c r="H40" s="49"/>
+      <c r="I40" s="107"/>
+      <c r="J40" s="108"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="44"/>
-      <c r="C41" s="45"/>
-      <c r="D41" s="45"/>
-      <c r="E41" s="46"/>
-      <c r="F41" s="32"/>
-      <c r="G41" s="69"/>
-      <c r="H41" s="70"/>
-      <c r="I41" s="71"/>
-      <c r="J41" s="72"/>
+      <c r="B41" s="118"/>
+      <c r="C41" s="119"/>
+      <c r="D41" s="119"/>
+      <c r="E41" s="120"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="48"/>
+      <c r="H41" s="49"/>
+      <c r="I41" s="107"/>
+      <c r="J41" s="108"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="44"/>
-      <c r="C42" s="45"/>
-      <c r="D42" s="45"/>
-      <c r="E42" s="46"/>
-      <c r="F42" s="32"/>
-      <c r="G42" s="69"/>
-      <c r="H42" s="70"/>
-      <c r="I42" s="71"/>
-      <c r="J42" s="72"/>
+      <c r="B42" s="118"/>
+      <c r="C42" s="119"/>
+      <c r="D42" s="119"/>
+      <c r="E42" s="120"/>
+      <c r="F42" s="30"/>
+      <c r="G42" s="48"/>
+      <c r="H42" s="49"/>
+      <c r="I42" s="107"/>
+      <c r="J42" s="108"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B43" s="44"/>
-      <c r="C43" s="45"/>
-      <c r="D43" s="45"/>
-      <c r="E43" s="46"/>
-      <c r="F43" s="32"/>
-      <c r="G43" s="69"/>
-      <c r="H43" s="70"/>
-      <c r="I43" s="71"/>
-      <c r="J43" s="72"/>
+      <c r="B43" s="118"/>
+      <c r="C43" s="119"/>
+      <c r="D43" s="119"/>
+      <c r="E43" s="120"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="48"/>
+      <c r="H43" s="49"/>
+      <c r="I43" s="107"/>
+      <c r="J43" s="108"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B44" s="44"/>
-      <c r="C44" s="45"/>
-      <c r="D44" s="45"/>
-      <c r="E44" s="46"/>
-      <c r="F44" s="32"/>
-      <c r="G44" s="69"/>
-      <c r="H44" s="70"/>
-      <c r="I44" s="71"/>
-      <c r="J44" s="72"/>
+      <c r="B44" s="118"/>
+      <c r="C44" s="119"/>
+      <c r="D44" s="119"/>
+      <c r="E44" s="120"/>
+      <c r="F44" s="30"/>
+      <c r="G44" s="48"/>
+      <c r="H44" s="49"/>
+      <c r="I44" s="107"/>
+      <c r="J44" s="108"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B45" s="44"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="46"/>
-      <c r="F45" s="32"/>
-      <c r="G45" s="69"/>
-      <c r="H45" s="70"/>
-      <c r="I45" s="71"/>
-      <c r="J45" s="72"/>
+      <c r="B45" s="118"/>
+      <c r="C45" s="119"/>
+      <c r="D45" s="119"/>
+      <c r="E45" s="120"/>
+      <c r="F45" s="30"/>
+      <c r="G45" s="48"/>
+      <c r="H45" s="49"/>
+      <c r="I45" s="107"/>
+      <c r="J45" s="108"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B46" s="44"/>
-      <c r="C46" s="45"/>
-      <c r="D46" s="45"/>
-      <c r="E46" s="46"/>
-      <c r="F46" s="32"/>
-      <c r="G46" s="69"/>
-      <c r="H46" s="70"/>
-      <c r="I46" s="71"/>
-      <c r="J46" s="72"/>
+      <c r="B46" s="118"/>
+      <c r="C46" s="119"/>
+      <c r="D46" s="119"/>
+      <c r="E46" s="120"/>
+      <c r="F46" s="30"/>
+      <c r="G46" s="48"/>
+      <c r="H46" s="49"/>
+      <c r="I46" s="107"/>
+      <c r="J46" s="108"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B47" s="44"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="46"/>
-      <c r="F47" s="32"/>
-      <c r="G47" s="69"/>
-      <c r="H47" s="70"/>
-      <c r="I47" s="71"/>
-      <c r="J47" s="72"/>
+      <c r="B47" s="118"/>
+      <c r="C47" s="119"/>
+      <c r="D47" s="119"/>
+      <c r="E47" s="120"/>
+      <c r="F47" s="30"/>
+      <c r="G47" s="48"/>
+      <c r="H47" s="49"/>
+      <c r="I47" s="107"/>
+      <c r="J47" s="108"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B48" s="47"/>
-      <c r="C48" s="48"/>
-      <c r="D48" s="48"/>
-      <c r="E48" s="49"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="69"/>
-      <c r="H48" s="70"/>
+      <c r="B48" s="121"/>
+      <c r="C48" s="122"/>
+      <c r="D48" s="122"/>
+      <c r="E48" s="123"/>
+      <c r="F48" s="30"/>
+      <c r="G48" s="48"/>
+      <c r="H48" s="49"/>
       <c r="I48" s="73"/>
-      <c r="J48" s="74"/>
+      <c r="J48" s="75"/>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B49" s="4"/>
@@ -1783,12 +1782,12 @@
       <c r="F49" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G49" s="121" t="s">
+      <c r="G49" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="H49" s="122"/>
-      <c r="I49" s="75"/>
-      <c r="J49" s="76"/>
+      <c r="H49" s="51"/>
+      <c r="I49" s="93"/>
+      <c r="J49" s="94"/>
     </row>
     <row r="50" spans="2:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B50" s="4"/>
@@ -1796,10 +1795,10 @@
       <c r="D50" s="19"/>
       <c r="E50" s="2"/>
       <c r="F50" s="20"/>
-      <c r="G50" s="123"/>
-      <c r="H50" s="124"/>
-      <c r="I50" s="77"/>
-      <c r="J50" s="78"/>
+      <c r="G50" s="52"/>
+      <c r="H50" s="53"/>
+      <c r="I50" s="95"/>
+      <c r="J50" s="96"/>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B51" s="6"/>
@@ -1807,63 +1806,163 @@
       <c r="D51" s="8"/>
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
-      <c r="G51" s="59"/>
-      <c r="H51" s="60"/>
-      <c r="I51" s="79"/>
-      <c r="J51" s="80"/>
+      <c r="G51" s="109"/>
+      <c r="H51" s="110"/>
+      <c r="I51" s="97"/>
+      <c r="J51" s="98"/>
     </row>
     <row r="52" spans="2:10" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B52" s="24"/>
-      <c r="C52" s="25"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="25"/>
+      <c r="B52" s="22"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="23"/>
       <c r="F52" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G52" s="61" t="s">
+      <c r="G52" s="111" t="s">
         <v>20</v>
       </c>
-      <c r="H52" s="62"/>
-      <c r="I52" s="81"/>
-      <c r="J52" s="82"/>
+      <c r="H52" s="112"/>
+      <c r="I52" s="99"/>
+      <c r="J52" s="100"/>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B53" s="50" t="s">
+      <c r="B53" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="C53" s="51"/>
-      <c r="D53" s="51"/>
-      <c r="E53" s="52"/>
-      <c r="F53" s="23"/>
-      <c r="G53" s="51"/>
-      <c r="H53" s="52"/>
-      <c r="I53" s="50"/>
-      <c r="J53" s="52"/>
+      <c r="C53" s="113"/>
+      <c r="D53" s="113"/>
+      <c r="E53" s="102"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="113"/>
+      <c r="H53" s="102"/>
+      <c r="I53" s="101"/>
+      <c r="J53" s="102"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B54" s="53"/>
-      <c r="C54" s="54"/>
-      <c r="D54" s="54"/>
-      <c r="E54" s="55"/>
-      <c r="F54" s="21"/>
-      <c r="G54" s="111"/>
-      <c r="H54" s="112"/>
-      <c r="I54" s="115"/>
-      <c r="J54" s="116"/>
+      <c r="B54" s="124"/>
+      <c r="C54" s="125"/>
+      <c r="D54" s="125"/>
+      <c r="E54" s="126"/>
+      <c r="F54" s="134"/>
+      <c r="G54" s="132"/>
+      <c r="H54" s="133"/>
+      <c r="I54" s="42"/>
+      <c r="J54" s="43"/>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B55" s="56"/>
-      <c r="C55" s="57"/>
-      <c r="D55" s="57"/>
-      <c r="E55" s="58"/>
-      <c r="F55" s="22"/>
-      <c r="G55" s="113"/>
-      <c r="H55" s="114"/>
-      <c r="I55" s="117"/>
-      <c r="J55" s="118"/>
+      <c r="B55" s="127"/>
+      <c r="C55" s="128"/>
+      <c r="D55" s="128"/>
+      <c r="E55" s="129"/>
+      <c r="F55" s="135"/>
+      <c r="G55" s="130"/>
+      <c r="H55" s="131"/>
+      <c r="I55" s="44"/>
+      <c r="J55" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="124">
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="B54:E55"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="B46:E46"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="I52:J52"/>
+    <mergeCell ref="I53:J53"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="E2:J4"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="H11:J12"/>
+    <mergeCell ref="B2:D4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
     <mergeCell ref="G54:H54"/>
     <mergeCell ref="G55:H55"/>
     <mergeCell ref="I54:J54"/>
@@ -1888,106 +1987,6 @@
     <mergeCell ref="G48:H48"/>
     <mergeCell ref="G49:H49"/>
     <mergeCell ref="G50:H50"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="E2:J4"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="H11:J12"/>
-    <mergeCell ref="B2:D4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="I49:J49"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="I51:J51"/>
-    <mergeCell ref="I52:J52"/>
-    <mergeCell ref="I53:J53"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I48:J48"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="B48:E48"/>
-    <mergeCell ref="B53:E53"/>
-    <mergeCell ref="B54:E55"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="B46:E46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>